<commit_message>
added consolidated files and revised website source
</commit_message>
<xml_diff>
--- a/Website Source.xlsx
+++ b/Website Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\18. Project 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\18. Project 2\Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5955391-3298-415F-9805-F8008362ACB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC3FCE-E388-4D4E-8DAE-6DB0D3550B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1906FD7-D1DF-497F-A237-2FEC0712D0CC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{E1906FD7-D1DF-497F-A237-2FEC0712D0CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Topic</t>
   </si>
@@ -134,6 +134,25 @@
   </si>
   <si>
     <t>New data on Volunteering in Australia - Oct 2020</t>
+  </si>
+  <si>
+    <t>https://inaturalist.ala.org.au/observations/export?projects%5B%5D=environment-recovery-project</t>
+  </si>
+  <si>
+    <t>https://www.agriculture.gov.au/abares/forestsaustralia/forest-data-maps-and-tools</t>
+  </si>
+  <si>
+    <t>https://www.environment.gov.au/fed/catalog/search/resource/details.page?uuid=%7B9ACDCB09-0364-4FE8-9459-2A56C792C743%7D</t>
+  </si>
+  <si>
+    <t>Environment Recovery Project</t>
+  </si>
+  <si>
+    <t>Forest data, maps and tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+National Indicative Aggregated Fire Extent Datasets</t>
   </si>
 </sst>
 </file>
@@ -225,13 +244,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,15 +566,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A1EE92-D606-407E-9143-7B1E91BFA36B}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -591,7 +610,7 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1"/>
@@ -673,11 +692,35 @@
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="6"/>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -690,9 +733,10 @@
     <hyperlink ref="B8" r:id="rId7" xr:uid="{E13F375F-9AE5-40EC-AEA4-7BF7CE551758}"/>
     <hyperlink ref="B9" r:id="rId8" xr:uid="{7501568E-CC51-49EC-B355-FBF147DE1CCC}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{D1292534-CF04-4F66-AFF4-82F8ACEE8A1D}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{D30AEFA3-B782-4D6C-AFD4-83C346661A35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>